<commit_message>
updated models with local
</commit_message>
<xml_diff>
--- a/forecast/china/Attribute_and_data_points.xlsx
+++ b/forecast/china/Attribute_and_data_points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stemly.sharepoint.com/sites/Customer-FAB/Shared Documents/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{2B23679A-F5C0-40B3-AE01-8457D549CD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92BF83B3-19CA-48E0-B985-F9A633448673}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8_{2B23679A-F5C0-40B3-AE01-8457D549CD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECF28B4B-F777-4EC7-B84E-B92FFDCE1645}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1545" windowWidth="29040" windowHeight="15720" xr2:uid="{45EF6ED3-064D-488E-A779-6C19942B5000}"/>
+    <workbookView minimized="1" xWindow="-28800" yWindow="255" windowWidth="14340" windowHeight="7245" xr2:uid="{45EF6ED3-064D-488E-A779-6C19942B5000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes_China" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="129">
   <si>
     <t>SKU Description</t>
   </si>
@@ -462,9 +462,6 @@
     <t>Oil Control Pads 28 pcs</t>
   </si>
   <si>
-    <t>Not found please neglect</t>
-  </si>
-  <si>
     <t>Oatmeal Mask 2oz</t>
   </si>
   <si>
@@ -490,13 +487,16 @@
   </si>
   <si>
     <t>URC 2oz Jar</t>
+  </si>
+  <si>
+    <t>Face cleanser 5oz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,6 +545,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -805,7 +812,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -859,6 +866,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1198,7 +1206,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1236,7 +1244,7 @@
         <v>41</v>
       </c>
       <c r="I1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1262,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I2">
         <v>82314745</v>
@@ -1349,7 +1357,7 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I5">
         <v>82314724</v>
@@ -1465,7 +1473,7 @@
         <v>22</v>
       </c>
       <c r="H9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I9">
         <v>82314725</v>
@@ -1523,7 +1531,7 @@
         <v>28</v>
       </c>
       <c r="H11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I11">
         <v>80685834</v>
@@ -1552,7 +1560,7 @@
         <v>22</v>
       </c>
       <c r="H12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I12">
         <v>80685602</v>
@@ -1638,8 +1646,8 @@
       <c r="G15" t="s">
         <v>22</v>
       </c>
-      <c r="H15" t="s">
-        <v>119</v>
+      <c r="H15" s="31" t="s">
+        <v>128</v>
       </c>
       <c r="I15">
         <v>80693598</v>
@@ -1668,7 +1676,7 @@
         <v>22</v>
       </c>
       <c r="H16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I16">
         <v>80693877</v>
@@ -1697,7 +1705,7 @@
         <v>35</v>
       </c>
       <c r="H17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I17">
         <v>80703071</v>
@@ -1726,7 +1734,7 @@
         <v>10</v>
       </c>
       <c r="H18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I18">
         <v>82314747</v>
@@ -1776,7 +1784,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:F13"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1861,6 +1869,9 @@
       </c>
       <c r="F3">
         <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
       </c>
       <c r="H3" t="s">
         <v>45</v>
@@ -2548,26 +2559,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="da21cd1a-3dfe-4f9c-a347-c59b2585430e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f56a5b06-0ec5-418f-a114-0aff6503796d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ABCB688460B1EF42B10F48AE8F333763" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2a21087f131ac4c977f0f32ad26008e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f56a5b06-0ec5-418f-a114-0aff6503796d" xmlns:ns3="da21cd1a-3dfe-4f9c-a347-c59b2585430e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c1b31aa21244abb472c445538e18a6a" ns2:_="" ns3:_="">
     <xsd:import namespace="f56a5b06-0ec5-418f-a114-0aff6503796d"/>
@@ -2744,26 +2735,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{550DE15A-D704-41B4-A4F1-B16CBBD5D54B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="da21cd1a-3dfe-4f9c-a347-c59b2585430e"/>
-    <ds:schemaRef ds:uri="f56a5b06-0ec5-418f-a114-0aff6503796d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{064BAE1A-4D0B-44A1-B9E7-6DA1E76148A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="da21cd1a-3dfe-4f9c-a347-c59b2585430e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f56a5b06-0ec5-418f-a114-0aff6503796d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E555BE74-ED75-4615-8F2C-B2F4036C019E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2780,4 +2772,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{064BAE1A-4D0B-44A1-B9E7-6DA1E76148A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{550DE15A-D704-41B4-A4F1-B16CBBD5D54B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="da21cd1a-3dfe-4f9c-a347-c59b2585430e"/>
+    <ds:schemaRef ds:uri="f56a5b06-0ec5-418f-a114-0aff6503796d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>